<commit_message>
Repurpose geothermal as pumped hydro
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\elec\BDSBaPCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B789F-318E-4614-B038-8750D7B201AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -160,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -297,23 +296,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -349,23 +331,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,21 +506,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -563,112 +528,112 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -679,28 +644,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" customWidth="1"/>
+    <col min="2" max="2" width="23.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -708,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -716,7 +681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -724,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -732,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -740,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -748,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -756,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -764,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -772,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -780,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -788,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -797,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -806,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -815,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -824,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>35</v>
       </c>

</xml_diff>